<commit_message>
added another operation in TC 4 and added the TC 5
</commit_message>
<xml_diff>
--- a/HybridFramework_October/TestData/Data.xlsx
+++ b/HybridFramework_October/TestData/Data.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2BF92F-C601-49B3-A6C2-9D7DE3BEFB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SauceLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="webshop" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -29,12 +30,18 @@
   <si>
     <t>secret_sauce</t>
   </si>
+  <si>
+    <t>abhinavrevu16@gmail.com</t>
+  </si>
+  <si>
+    <t>Abhi@123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +63,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,19 +89,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -133,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,9 +191,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,6 +243,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -374,16 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -391,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -406,24 +468,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{088C20A4-3957-4886-A39A-C5C209EC7A15}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{40C65060-2FD7-4F56-8793-378848BC312E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>